<commit_message>
Better scale circles on map.
</commit_message>
<xml_diff>
--- a/data/stasj_lat_lon.xlsx
+++ b/data/stasj_lat_lon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/elianne_egge_niva_no/Documents/qPCR_heatmap/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/anette_engesmo_niva_no/Documents/Delte dokumenter og mapper/Pukkellaks manuskript eDNA/200130_fish_eDNA_rscripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{91454F38-772B-4405-848A-F3CED5CA996A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CAA7B3B5-2F9B-4CC8-9544-CA0CC4A533FF}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{91454F38-772B-4405-848A-F3CED5CA996A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0484133B-174C-4929-8DFB-16E260618F8C}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1490" windowWidth="14400" windowHeight="7360" xr2:uid="{5963E4D2-A413-4848-ABD2-BCD71A2918CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5963E4D2-A413-4848-ABD2-BCD71A2918CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,23 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,22 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDB86FF-F057-4714-8322-8E08D0FCB463}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D24"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="8.7265625" style="5"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
@@ -510,11 +496,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
@@ -529,12 +515,24 @@
       <c r="F2" s="2">
         <v>30.9377</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>24.1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>69.646569999999997</v>
+      </c>
+      <c r="L2" s="2">
+        <v>30.9377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3">
@@ -549,12 +547,24 @@
       <c r="F3" s="2">
         <v>30.939630000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>19.8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>69.675269999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>30.939630000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4">
@@ -569,12 +579,24 @@
       <c r="F4" s="2">
         <v>30.891089999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>13.8</v>
+      </c>
+      <c r="K4" s="1">
+        <v>69.703220000000002</v>
+      </c>
+      <c r="L4" s="2">
+        <v>30.891089999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5">
@@ -589,12 +611,24 @@
       <c r="F5" s="2">
         <v>30.887350000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2">
+        <v>69.724459999999993</v>
+      </c>
+      <c r="L5" s="2">
+        <v>30.887350000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
@@ -609,12 +643,24 @@
       <c r="F6" s="2">
         <v>30.952200000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>28.1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>69.615120000000005</v>
+      </c>
+      <c r="L6" s="2">
+        <v>30.952200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7">
@@ -629,12 +675,24 @@
       <c r="F7" s="2">
         <v>30.94154</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>32</v>
+      </c>
+      <c r="K7" s="2">
+        <v>69.582909999999998</v>
+      </c>
+      <c r="L7" s="2">
+        <v>30.94154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
@@ -643,18 +701,18 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <v>77.95993</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="2">
         <v>14.26745</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -663,18 +721,18 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>78.271820000000005</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>13.77031</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
@@ -683,290 +741,290 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>80.284080000000003</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>22.59281</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
         <v>59.13147</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="2">
         <v>10.19806</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
         <v>59.128929999999997</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="2">
         <v>10.20167</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
         <v>59.127400000000002</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="2">
         <v>10.20224</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
         <v>59.124139999999997</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="2">
         <v>10.201589999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
         <v>59.105800000000002</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="2">
         <v>10.20518</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="11">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
         <v>59.105539999999998</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="2">
         <v>10.20091</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21">
         <v>7</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="11">
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
         <v>59.094769999999997</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="2">
         <v>10.203010000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
         <v>8</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="11">
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
         <v>59.073430000000002</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="2">
         <v>10.184100000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="10">
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
         <v>59.079889999999999</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="1">
         <v>10.20241</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="11">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
         <v>59.079410000000003</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="2">
         <v>10.202590000000001</v>
       </c>
     </row>

</xml_diff>